<commit_message>
update to variable map
</commit_message>
<xml_diff>
--- a/Study Metadata Variable Map.xlsx
+++ b/Study Metadata Variable Map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\steph\Documents\GitHub\2020-07-Growth-Database\Vinh_growth_database\Metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\2020_04\Pig-database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E791274-BAF8-426D-BF28-E10F6C7EA1CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6C1EDB-4ACD-413B-AAF0-2886244DAE23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-1848" windowWidth="30936" windowHeight="17040" xr2:uid="{8502223F-7BAC-4135-A94A-571E25FE319D}"/>
+    <workbookView xWindow="24900" yWindow="9765" windowWidth="28800" windowHeight="15435" xr2:uid="{8502223F-7BAC-4135-A94A-571E25FE319D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="121">
   <si>
     <t>Variable</t>
   </si>
@@ -76,9 +76,6 @@
     <t>treatment</t>
   </si>
   <si>
-    <t>Uninhibited/Inhibited</t>
-  </si>
-  <si>
     <t>antibiotics</t>
   </si>
   <si>
@@ -251,13 +248,163 @@
   </si>
   <si>
     <t>Whether males (M), females (F), or both (FM) were included in the study</t>
+  </si>
+  <si>
+    <t>Source.Name</t>
+  </si>
+  <si>
+    <t>Identifier</t>
+  </si>
+  <si>
+    <t>PND</t>
+  </si>
+  <si>
+    <t>BW</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Rearing</t>
+  </si>
+  <si>
+    <t>Brain Wt (g)</t>
+  </si>
+  <si>
+    <t>Intestinal Wt (g)</t>
+  </si>
+  <si>
+    <t>Lung Wt (g)</t>
+  </si>
+  <si>
+    <t>Heart Wt (g)</t>
+  </si>
+  <si>
+    <t>Kidneys Wt (g)</t>
+  </si>
+  <si>
+    <t>Spleen Wt (g)</t>
+  </si>
+  <si>
+    <t>Liver Wt (g)</t>
+  </si>
+  <si>
+    <t>PercentBrain</t>
+  </si>
+  <si>
+    <t>PercentIntestine</t>
+  </si>
+  <si>
+    <t>PercentLung</t>
+  </si>
+  <si>
+    <t>PercentHeart</t>
+  </si>
+  <si>
+    <t>PercentKidneys</t>
+  </si>
+  <si>
+    <t>PercentSpleen</t>
+  </si>
+  <si>
+    <t>PercentLiver</t>
+  </si>
+  <si>
+    <t>Feedingstyles</t>
+  </si>
+  <si>
+    <t>Investigator</t>
+  </si>
+  <si>
+    <t>Institution</t>
+  </si>
+  <si>
+    <t>Name of the reviewer assigned for the study</t>
+  </si>
+  <si>
+    <t>Identification for the source of the study</t>
+  </si>
+  <si>
+    <t>Identification for the source of the study follow by the animal identifier</t>
+  </si>
+  <si>
+    <t>Post natal day</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>Body weight</t>
+  </si>
+  <si>
+    <t>Kg</t>
+  </si>
+  <si>
+    <t>Sex of the pig</t>
+  </si>
+  <si>
+    <t>Rearing style of the pig</t>
+  </si>
+  <si>
+    <t>Brain organ weight</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>Intestinal organ weight</t>
+  </si>
+  <si>
+    <t>Lung organ weight</t>
+  </si>
+  <si>
+    <t>Kidneys organ weight</t>
+  </si>
+  <si>
+    <t>Spleen organ weight</t>
+  </si>
+  <si>
+    <t>Liver organ weight</t>
+  </si>
+  <si>
+    <t>Hear organ weight</t>
+  </si>
+  <si>
+    <t>Brain weight as percent of total body weight</t>
+  </si>
+  <si>
+    <t>Intestine weight as percent of total body weight</t>
+  </si>
+  <si>
+    <t>Lung weight as percent of total body weight</t>
+  </si>
+  <si>
+    <t>Heart weight as percent of total body weight</t>
+  </si>
+  <si>
+    <t>Kidneys weight as percent of total body weight</t>
+  </si>
+  <si>
+    <t>Spleen weight as percent of total body weight</t>
+  </si>
+  <si>
+    <t>Liver weight as percent of total body weight</t>
+  </si>
+  <si>
+    <t>Feeding styles, adlibitum or custom for each pig</t>
+  </si>
+  <si>
+    <t>the principal investigator for each study</t>
+  </si>
+  <si>
+    <t>the instituion where the study was performed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,6 +420,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -282,7 +435,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -308,11 +461,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -324,6 +514,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -639,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EABD5131-AD43-46E0-9736-B34083590A23}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C2:C5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,7 +865,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -677,7 +873,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -685,23 +881,23 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -709,10 +905,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -720,10 +916,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -731,10 +927,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -742,10 +938,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -753,7 +949,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -761,7 +957,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -769,13 +965,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -811,7 +1010,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>46</v>
@@ -827,10 +1026,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -851,7 +1050,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>53</v>
@@ -859,21 +1058,24 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>54</v>
       </c>
+      <c r="C25" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>63</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -884,7 +1086,7 @@
         <v>56</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -906,7 +1108,7 @@
         <v>58</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -917,32 +1119,301 @@
         <v>59</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>23</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B53" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B54" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" s="9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="7"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="7"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="7"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="7"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="7"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="7"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="7"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>